<commit_message>
font ve renk biçimlendirme
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,13 +32,37 @@
       <sz val="16"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="002C27CB"/>
+      <sz val="16"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0027CB5B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E3331B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0008D84A"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -53,11 +77,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -576,9 +605,9 @@
           <t>Final</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ortalama</t>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Ortalama</t>
         </is>
       </c>
     </row>
@@ -594,7 +623,7 @@
       <c r="C2" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="7" t="n">
         <v>55</v>
       </c>
     </row>
@@ -610,7 +639,7 @@
       <c r="C3" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="8" t="n">
         <v>82.5</v>
       </c>
     </row>
@@ -626,7 +655,7 @@
       <c r="C4" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="8" t="n">
         <v>85</v>
       </c>
     </row>
@@ -642,7 +671,7 @@
       <c r="C5" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="7" t="n">
         <v>67.5</v>
       </c>
     </row>

</xml_diff>